<commit_message>
HOP-2914: split compose files and make tests more modular
</commit_message>
<xml_diff>
--- a/integration-tests/spreadsheet/files/exelwriter-testfile.xlsx
+++ b/integration-tests/spreadsheet/files/exelwriter-testfile.xlsx
@@ -20,64 +20,64 @@
     <t>number</t>
   </si>
   <si>
-    <t>Tenesha Pfeffer</t>
-  </si>
-  <si>
-    <t>3541703</t>
-  </si>
-  <si>
-    <t>Cherilyn Pfannerstill</t>
-  </si>
-  <si>
-    <t>966960</t>
-  </si>
-  <si>
-    <t>Mrs. Thad Murray</t>
-  </si>
-  <si>
-    <t>5623823</t>
-  </si>
-  <si>
-    <t>Yasmine Toy IV</t>
-  </si>
-  <si>
-    <t>855</t>
-  </si>
-  <si>
-    <t>Ms. Nelly Koelpin</t>
-  </si>
-  <si>
-    <t>782258867</t>
-  </si>
-  <si>
-    <t>Mrs. Tory McCullough</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Wilford Runte</t>
-  </si>
-  <si>
-    <t>63560715</t>
-  </si>
-  <si>
-    <t>Adriane McLaughlin</t>
-  </si>
-  <si>
-    <t>916</t>
-  </si>
-  <si>
-    <t>Rhona Reilly</t>
-  </si>
-  <si>
-    <t>1008653</t>
-  </si>
-  <si>
-    <t>Terry Huels</t>
-  </si>
-  <si>
-    <t>49887</t>
+    <t>Homer Purdy</t>
+  </si>
+  <si>
+    <t>509</t>
+  </si>
+  <si>
+    <t>Joella Hansen</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>Buford Kuhn</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Dr. Antonia Johns</t>
+  </si>
+  <si>
+    <t>635</t>
+  </si>
+  <si>
+    <t>Randa Carroll</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Darrin Stanton</t>
+  </si>
+  <si>
+    <t>64333570</t>
+  </si>
+  <si>
+    <t>Pearlene Jacobs</t>
+  </si>
+  <si>
+    <t>6607</t>
+  </si>
+  <si>
+    <t>Normand Morissette</t>
+  </si>
+  <si>
+    <t>2089</t>
+  </si>
+  <si>
+    <t>Shanna Rowe Sr.</t>
+  </si>
+  <si>
+    <t>39009042</t>
+  </si>
+  <si>
+    <t>Russell Walsh</t>
+  </si>
+  <si>
+    <t>9449</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
HOP-2914: fix containers on jenkins
</commit_message>
<xml_diff>
--- a/integration-tests/spreadsheet/files/exelwriter-testfile.xlsx
+++ b/integration-tests/spreadsheet/files/exelwriter-testfile.xlsx
@@ -20,64 +20,64 @@
     <t>number</t>
   </si>
   <si>
-    <t>Homer Purdy</t>
-  </si>
-  <si>
-    <t>509</t>
-  </si>
-  <si>
-    <t>Joella Hansen</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>Buford Kuhn</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Dr. Antonia Johns</t>
-  </si>
-  <si>
-    <t>635</t>
-  </si>
-  <si>
-    <t>Randa Carroll</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>Darrin Stanton</t>
-  </si>
-  <si>
-    <t>64333570</t>
-  </si>
-  <si>
-    <t>Pearlene Jacobs</t>
-  </si>
-  <si>
-    <t>6607</t>
-  </si>
-  <si>
-    <t>Normand Morissette</t>
-  </si>
-  <si>
-    <t>2089</t>
-  </si>
-  <si>
-    <t>Shanna Rowe Sr.</t>
-  </si>
-  <si>
-    <t>39009042</t>
-  </si>
-  <si>
-    <t>Russell Walsh</t>
-  </si>
-  <si>
-    <t>9449</t>
+    <t>Mrs. Cherlyn Doyle</t>
+  </si>
+  <si>
+    <t>1702</t>
+  </si>
+  <si>
+    <t>Numbers Ryan</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Branda Emmerich</t>
+  </si>
+  <si>
+    <t>411073826</t>
+  </si>
+  <si>
+    <t>Simon Hintz</t>
+  </si>
+  <si>
+    <t>44525821</t>
+  </si>
+  <si>
+    <t>Oswaldo Macejkovic</t>
+  </si>
+  <si>
+    <t>26351692</t>
+  </si>
+  <si>
+    <t>Juanita Schiller</t>
+  </si>
+  <si>
+    <t>911</t>
+  </si>
+  <si>
+    <t>Elia Adams</t>
+  </si>
+  <si>
+    <t>914526</t>
+  </si>
+  <si>
+    <t>Lynn Thompson III</t>
+  </si>
+  <si>
+    <t>2823995</t>
+  </si>
+  <si>
+    <t>Olen Wolff</t>
+  </si>
+  <si>
+    <t>5860787</t>
+  </si>
+  <si>
+    <t>Dr. Jim Pollich</t>
+  </si>
+  <si>
+    <t>979903</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
HOP-2914: update integration testing to be more modular (#845)
* HOP-2914: split compose files and make tests more modular

* HOP-2914: fix containers on jenkins

* HOP-2914: add build args to custom images

* HOP-2914: add args

* HOP-2914: fix variables

* HOP-2914: update docs and enable full build again
</commit_message>
<xml_diff>
--- a/integration-tests/spreadsheet/files/exelwriter-testfile.xlsx
+++ b/integration-tests/spreadsheet/files/exelwriter-testfile.xlsx
@@ -20,64 +20,64 @@
     <t>number</t>
   </si>
   <si>
-    <t>Tenesha Pfeffer</t>
-  </si>
-  <si>
-    <t>3541703</t>
-  </si>
-  <si>
-    <t>Cherilyn Pfannerstill</t>
-  </si>
-  <si>
-    <t>966960</t>
-  </si>
-  <si>
-    <t>Mrs. Thad Murray</t>
-  </si>
-  <si>
-    <t>5623823</t>
-  </si>
-  <si>
-    <t>Yasmine Toy IV</t>
-  </si>
-  <si>
-    <t>855</t>
-  </si>
-  <si>
-    <t>Ms. Nelly Koelpin</t>
-  </si>
-  <si>
-    <t>782258867</t>
-  </si>
-  <si>
-    <t>Mrs. Tory McCullough</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Wilford Runte</t>
-  </si>
-  <si>
-    <t>63560715</t>
-  </si>
-  <si>
-    <t>Adriane McLaughlin</t>
-  </si>
-  <si>
-    <t>916</t>
-  </si>
-  <si>
-    <t>Rhona Reilly</t>
-  </si>
-  <si>
-    <t>1008653</t>
-  </si>
-  <si>
-    <t>Terry Huels</t>
-  </si>
-  <si>
-    <t>49887</t>
+    <t>Mrs. Cherlyn Doyle</t>
+  </si>
+  <si>
+    <t>1702</t>
+  </si>
+  <si>
+    <t>Numbers Ryan</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Branda Emmerich</t>
+  </si>
+  <si>
+    <t>411073826</t>
+  </si>
+  <si>
+    <t>Simon Hintz</t>
+  </si>
+  <si>
+    <t>44525821</t>
+  </si>
+  <si>
+    <t>Oswaldo Macejkovic</t>
+  </si>
+  <si>
+    <t>26351692</t>
+  </si>
+  <si>
+    <t>Juanita Schiller</t>
+  </si>
+  <si>
+    <t>911</t>
+  </si>
+  <si>
+    <t>Elia Adams</t>
+  </si>
+  <si>
+    <t>914526</t>
+  </si>
+  <si>
+    <t>Lynn Thompson III</t>
+  </si>
+  <si>
+    <t>2823995</t>
+  </si>
+  <si>
+    <t>Olen Wolff</t>
+  </si>
+  <si>
+    <t>5860787</t>
+  </si>
+  <si>
+    <t>Dr. Jim Pollich</t>
+  </si>
+  <si>
+    <t>979903</t>
   </si>
 </sst>
 </file>

</xml_diff>